<commit_message>
lab5: add 30mm offset to inner and outer ring textfiles
</commit_message>
<xml_diff>
--- a/lab5/trajectories/helpers/trajectory_visualization.xlsx
+++ b/lab5/trajectories/helpers/trajectory_visualization.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://unaledu-my.sharepoint.com/personal/jhgallego_unal_edu_co/Documents/Documents/UNAL Docs/2022-II/Robótica/git repo/robotics_unal/lab5/trajectories/helpers/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="451" documentId="8_{0D532E6E-347B-40D2-8568-428AED43A9C2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{FC0FF3C2-83E3-4888-81D0-F7239C4F28C4}"/>
+  <xr:revisionPtr revIDLastSave="869" documentId="8_{0D532E6E-347B-40D2-8568-428AED43A9C2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{8D381F38-9AD7-42CB-B1CB-9B1FCDC0C41C}"/>
   <bookViews>
-    <workbookView xWindow="20280" yWindow="-15" windowWidth="20730" windowHeight="11160" tabRatio="862" activeTab="1" xr2:uid="{214E42D4-2653-4665-AEE6-D803265ECF39}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20640" windowHeight="11160" tabRatio="862" activeTab="6" xr2:uid="{214E42D4-2653-4665-AEE6-D803265ECF39}"/>
   </bookViews>
   <sheets>
     <sheet name="Circle" sheetId="2" r:id="rId1"/>
@@ -41,6 +41,41 @@
     </ext>
   </extLst>
 </workbook>
+</file>
+
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="105" uniqueCount="10">
+  <si>
+    <t>x</t>
+  </si>
+  <si>
+    <t>y</t>
+  </si>
+  <si>
+    <t>z</t>
+  </si>
+  <si>
+    <t>x2</t>
+  </si>
+  <si>
+    <t>y2</t>
+  </si>
+  <si>
+    <t>z2</t>
+  </si>
+  <si>
+    <t>r2</t>
+  </si>
+  <si>
+    <t>offset (mm)</t>
+  </si>
+  <si>
+    <t>offset(mm)</t>
+  </si>
+  <si>
+    <t>,</t>
+  </si>
+</sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
@@ -2288,7 +2323,7 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>inner_ring!$A$1:$A$33</c:f>
+              <c:f>inner_ring!$A$2:$A$34</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="33"/>
@@ -2393,7 +2428,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>inner_ring!$B$1:$B$33</c:f>
+              <c:f>inner_ring!$B$2:$B$34</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="33"/>
@@ -2500,6 +2535,349 @@
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000000-B943-458C-AEFE-60D207344020}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:v>series2</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent2"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>inner_ring!$F$2:$F$49</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="48"/>
+                <c:pt idx="0">
+                  <c:v>198</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>198</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>195.69975790000001</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>188.85247699999999</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>177.61725250000001</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>162.25513219999999</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>143.12305129999999</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>120.6655394</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>95.404391520000004</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>67.926544640000003</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>38.870440180000003</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>8.9111900469999998</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>8.9111900469999998</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>-8.9111900469999998</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>-38.870440180000003</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>-67.926544640000003</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>-95.404391520000004</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>-120.6655394</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>-143.12305129999999</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>-162.25513219999999</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>-177.61725250000001</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>-188.85247699999999</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>-195.69975790000001</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>-198</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>-198</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>-195.69975790000001</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>-188.85247699999999</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>-177.61725250000001</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>-162.25513219999999</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>-143.12305129999999</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>-120.6655394</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>-95.404391520000004</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>-67.926544640000003</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>-38.870440180000003</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>-8.9111900469999998</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>-8.9111900469999998</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>8.9111900469999998</c:v>
+                </c:pt>
+                <c:pt idx="37">
+                  <c:v>38.870440180000003</c:v>
+                </c:pt>
+                <c:pt idx="38">
+                  <c:v>67.926544640000003</c:v>
+                </c:pt>
+                <c:pt idx="39">
+                  <c:v>95.404391520000004</c:v>
+                </c:pt>
+                <c:pt idx="40">
+                  <c:v>120.6655394</c:v>
+                </c:pt>
+                <c:pt idx="41">
+                  <c:v>143.12305129999999</c:v>
+                </c:pt>
+                <c:pt idx="42">
+                  <c:v>162.25513219999999</c:v>
+                </c:pt>
+                <c:pt idx="43">
+                  <c:v>177.61725250000001</c:v>
+                </c:pt>
+                <c:pt idx="44">
+                  <c:v>188.85247699999999</c:v>
+                </c:pt>
+                <c:pt idx="45">
+                  <c:v>195.69975790000001</c:v>
+                </c:pt>
+                <c:pt idx="46">
+                  <c:v>198</c:v>
+                </c:pt>
+                <c:pt idx="47">
+                  <c:v>198</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>inner_ring!$H$2:$H$49</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="48"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>30.093267919999999</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>59.487325679999998</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>87.499209149999999</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>113.47806869999999</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>136.82029159999999</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>156.9835266</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>173.49928550000001</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>185.9838287</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>194.14708049999999</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>197.79936979999999</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>197.79936979999999</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>197.79936979999999</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>194.14708049999999</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>185.9838287</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>173.49928550000001</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>156.9835266</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>136.82029159999999</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>113.47806869999999</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>87.499209149999999</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>59.487325679999998</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>30.093267919999999</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>-30.093267919999999</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>-59.487325679999998</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>-87.499209149999999</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>-113.47806869999999</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>-136.82029159999999</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>-156.9835266</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>-173.49928550000001</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>-185.9838287</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>-194.14708049999999</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>-197.79936979999999</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>-197.79936979999999</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>-197.79936979999999</c:v>
+                </c:pt>
+                <c:pt idx="37">
+                  <c:v>-194.14708049999999</c:v>
+                </c:pt>
+                <c:pt idx="38">
+                  <c:v>-185.9838287</c:v>
+                </c:pt>
+                <c:pt idx="39">
+                  <c:v>-173.49928550000001</c:v>
+                </c:pt>
+                <c:pt idx="40">
+                  <c:v>-156.9835266</c:v>
+                </c:pt>
+                <c:pt idx="41">
+                  <c:v>-136.82029159999999</c:v>
+                </c:pt>
+                <c:pt idx="42">
+                  <c:v>-113.47806869999999</c:v>
+                </c:pt>
+                <c:pt idx="43">
+                  <c:v>-87.499209149999999</c:v>
+                </c:pt>
+                <c:pt idx="44">
+                  <c:v>-59.487325679999998</c:v>
+                </c:pt>
+                <c:pt idx="45">
+                  <c:v>-30.093267919999999</c:v>
+                </c:pt>
+                <c:pt idx="46">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="47">
+                  <c:v>0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-ED31-418C-8E6F-C3BFB56E5AEE}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -3346,7 +3724,7 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>outter_ring!$A$1:$A$44</c:f>
+              <c:f>outter_ring!$A$2:$A$45</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="44"/>
@@ -3487,7 +3865,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>outter_ring!$B$1:$B$44</c:f>
+              <c:f>outter_ring!$B$2:$B$45</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="44"/>
@@ -3630,6 +4008,325 @@
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000000-FC9C-455C-B064-D15A1328691E}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:v>SERIES3</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent2"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>outter_ring!$G$2:$G$45</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="44"/>
+                <c:pt idx="0">
+                  <c:v>265</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>265</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>260.02840455548545</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>245.30015981147619</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>221.36789125110025</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>221.36789125110025</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>189.12957287379737</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>149.79483395270174</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>104.83957190478087</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>55.95057447043088</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>4.9622289754635514</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>-4.9622289754635514</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>-55.95057447043088</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>-104.83957190478087</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>-149.79483395270174</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>-189.12957287379737</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>-189.12957287379737</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>-221.36789125110025</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>-245.30015981147619</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>-260.02840455548545</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>-265</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>-265</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>-265</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>-265</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>-260.02840455548545</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>-245.30015981147619</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>-221.36789125110025</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>-221.36789125110025</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>-189.12957287379737</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>-149.79483395270174</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>-104.83957190478087</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>-55.95057447043088</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>-4.9622289754635514</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>4.9622289750000004</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>55.950574469999999</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>104.8395719</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>149.79483400000001</c:v>
+                </c:pt>
+                <c:pt idx="37">
+                  <c:v>189.1295729</c:v>
+                </c:pt>
+                <c:pt idx="38">
+                  <c:v>189.1295729</c:v>
+                </c:pt>
+                <c:pt idx="39">
+                  <c:v>221.3678913</c:v>
+                </c:pt>
+                <c:pt idx="40">
+                  <c:v>245.30015979999999</c:v>
+                </c:pt>
+                <c:pt idx="41">
+                  <c:v>260.02840459999999</c:v>
+                </c:pt>
+                <c:pt idx="42">
+                  <c:v>265</c:v>
+                </c:pt>
+                <c:pt idx="43">
+                  <c:v>265</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>outter_ring!$H$2:$H$45</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="44"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>51.090398552262521</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>100.26381000234454</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>145.67517538415743</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>145.67517538415743</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>185.6205933200736</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>218.60125278872061</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>243.3796708089591</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>259.02612458287138</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>264.95353608399574</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>264.95353608399574</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>259.02612458287138</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>243.3796708089591</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>218.60125278872061</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>185.6205933200736</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>185.6205933200736</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>145.67517538415743</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>100.26381000234454</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>51.090398552262521</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>-51.090398550000003</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>-100.26381000000001</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>-145.6751754</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>-145.6751754</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>-185.6205933</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>-218.6012528</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>-243.37967080000001</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>-259.0261246</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>-264.95353610000001</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>-264.95353610000001</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>-259.0261246</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>-243.37967080000001</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>-218.6012528</c:v>
+                </c:pt>
+                <c:pt idx="37">
+                  <c:v>-185.6205933</c:v>
+                </c:pt>
+                <c:pt idx="38">
+                  <c:v>-185.6205933</c:v>
+                </c:pt>
+                <c:pt idx="39">
+                  <c:v>-145.6751754</c:v>
+                </c:pt>
+                <c:pt idx="40">
+                  <c:v>-100.26381000000001</c:v>
+                </c:pt>
+                <c:pt idx="41">
+                  <c:v>-51.090398550000003</c:v>
+                </c:pt>
+                <c:pt idx="42">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="43">
+                  <c:v>0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-8104-44CB-B537-57F463CB5FBA}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -9901,16 +10598,16 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>3</xdr:col>
-      <xdr:colOff>604837</xdr:colOff>
-      <xdr:row>0</xdr:row>
-      <xdr:rowOff>109537</xdr:rowOff>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>347662</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>166687</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>11</xdr:col>
-      <xdr:colOff>300037</xdr:colOff>
-      <xdr:row>14</xdr:row>
-      <xdr:rowOff>185737</xdr:rowOff>
+      <xdr:col>19</xdr:col>
+      <xdr:colOff>42862</xdr:colOff>
+      <xdr:row>16</xdr:row>
+      <xdr:rowOff>52387</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -9983,16 +10680,16 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>4</xdr:col>
-      <xdr:colOff>233362</xdr:colOff>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>585787</xdr:colOff>
       <xdr:row>1</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
+      <xdr:rowOff>47625</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>11</xdr:col>
-      <xdr:colOff>538162</xdr:colOff>
+      <xdr:col>21</xdr:col>
+      <xdr:colOff>280987</xdr:colOff>
       <xdr:row>15</xdr:row>
-      <xdr:rowOff>52387</xdr:rowOff>
+      <xdr:rowOff>100012</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -10604,7 +11301,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0DE71457-01A4-4D3C-84EC-76618EFC1FB4}">
   <dimension ref="A1:C53"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="N12" sqref="N12"/>
     </sheetView>
   </sheetViews>
@@ -11957,7 +12654,7 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7ECDB4BA-BFCF-4973-B0F5-DE3EBAE6E18E}">
-  <dimension ref="A1:C32"/>
+  <dimension ref="A1:J49"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="D9" sqref="D9"/>
@@ -11965,18 +12662,15 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A1">
-        <v>168</v>
-      </c>
-      <c r="B1">
-        <v>0</v>
-      </c>
-      <c r="C1">
-        <v>130</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="H1" t="s">
+        <v>8</v>
+      </c>
+      <c r="J1">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>168</v>
       </c>
@@ -11984,329 +12678,985 @@
         <v>0</v>
       </c>
       <c r="C2">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+        <v>130</v>
+      </c>
+      <c r="D2">
+        <f>COS(DEGREES(ATAN2(A2,B2)))*(SQRT(A2^2+B2^2)+$J$1)</f>
+        <v>198</v>
+      </c>
+      <c r="E2">
+        <f>SIN(DEGREES(ATAN2(A2,B2)))*(SQRT(A2^2+B2^2)+$J$1)</f>
+        <v>0</v>
+      </c>
+      <c r="F2">
+        <v>198</v>
+      </c>
+      <c r="G2" t="s">
+        <v>9</v>
+      </c>
+      <c r="H2">
+        <v>0</v>
+      </c>
+      <c r="I2" t="s">
+        <v>9</v>
+      </c>
+      <c r="J2">
+        <f>C2</f>
+        <v>130</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A3">
+        <v>168</v>
+      </c>
+      <c r="B3">
+        <v>0</v>
+      </c>
+      <c r="C3">
+        <v>0</v>
+      </c>
+      <c r="D3">
+        <f>COS(DEGREES(ATAN2(A3,B3)))*(SQRT(A3^2+B3^2)+$J$1)</f>
+        <v>198</v>
+      </c>
+      <c r="E3">
+        <f>SIN(DEGREES(ATAN2(A3,B3)))*(SQRT(A3^2+B3^2)+$J$1)</f>
+        <v>0</v>
+      </c>
+      <c r="F3">
+        <v>198</v>
+      </c>
+      <c r="G3" t="s">
+        <v>9</v>
+      </c>
+      <c r="H3">
+        <v>0</v>
+      </c>
+      <c r="I3" t="s">
+        <v>9</v>
+      </c>
+      <c r="J3">
+        <f t="shared" ref="J3:J49" si="0">C3</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A4">
         <v>164.072253359</v>
       </c>
-      <c r="B3">
+      <c r="B4">
         <v>-36.115033955000001</v>
       </c>
-      <c r="C3">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A4">
+      <c r="C4">
+        <v>0</v>
+      </c>
+      <c r="D4">
+        <f>COS(DEGREES(ATAN2(A4,B4)))*(SQRT(A4^2+B4^2)+$J$1)</f>
+        <v>195.6997578580409</v>
+      </c>
+      <c r="E4">
+        <f>SIN(DEGREES(ATAN2(A4,B4)))*(SQRT(A4^2+B4^2)+$J$1)</f>
+        <v>30.093267920778441</v>
+      </c>
+      <c r="F4">
+        <v>195.69975790000001</v>
+      </c>
+      <c r="G4" t="s">
+        <v>9</v>
+      </c>
+      <c r="H4">
+        <v>30.093267919999999</v>
+      </c>
+      <c r="I4" t="s">
+        <v>9</v>
+      </c>
+      <c r="J4">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A5">
         <v>152.472670505</v>
       </c>
-      <c r="B4">
+      <c r="B5">
         <v>-70.541369062000001</v>
       </c>
-      <c r="C4">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A5">
+      <c r="C5">
+        <v>0</v>
+      </c>
+      <c r="D5">
+        <f>COS(DEGREES(ATAN2(A5,B5)))*(SQRT(A5^2+B5^2)+$J$1)</f>
+        <v>188.85247703960047</v>
+      </c>
+      <c r="E5">
+        <f>SIN(DEGREES(ATAN2(A5,B5)))*(SQRT(A5^2+B5^2)+$J$1)</f>
+        <v>59.487325676036477</v>
+      </c>
+      <c r="F5">
+        <v>188.85247699999999</v>
+      </c>
+      <c r="G5" t="s">
+        <v>9</v>
+      </c>
+      <c r="H5">
+        <v>59.487325679999998</v>
+      </c>
+      <c r="I5" t="s">
+        <v>9</v>
+      </c>
+      <c r="J5">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A6">
         <v>133.743635039</v>
       </c>
-      <c r="B5">
+      <c r="B6">
         <v>-101.669268153</v>
       </c>
-      <c r="C5">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A6">
+      <c r="C6">
+        <v>0</v>
+      </c>
+      <c r="D6">
+        <f>COS(DEGREES(ATAN2(A6,B6)))*(SQRT(A6^2+B6^2)+$J$1)</f>
+        <v>177.61725253691722</v>
+      </c>
+      <c r="E6">
+        <f>SIN(DEGREES(ATAN2(A6,B6)))*(SQRT(A6^2+B6^2)+$J$1)</f>
+        <v>87.499209147778302</v>
+      </c>
+      <c r="F6">
+        <v>177.61725250000001</v>
+      </c>
+      <c r="G6" t="s">
+        <v>9</v>
+      </c>
+      <c r="H6">
+        <v>87.499209149999999</v>
+      </c>
+      <c r="I6" t="s">
+        <v>9</v>
+      </c>
+      <c r="J6">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A7">
         <v>108.760895843</v>
       </c>
-      <c r="B6">
+      <c r="B7">
         <v>-128.043225261</v>
       </c>
-      <c r="C6">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A7">
+      <c r="C7">
+        <v>0</v>
+      </c>
+      <c r="D7">
+        <f>COS(DEGREES(ATAN2(A7,B7)))*(SQRT(A7^2+B7^2)+$J$1)</f>
+        <v>162.25513217730688</v>
+      </c>
+      <c r="E7">
+        <f>SIN(DEGREES(ATAN2(A7,B7)))*(SQRT(A7^2+B7^2)+$J$1)</f>
+        <v>113.47806872652541</v>
+      </c>
+      <c r="F7">
+        <v>162.25513219999999</v>
+      </c>
+      <c r="G7" t="s">
+        <v>9</v>
+      </c>
+      <c r="H7">
+        <v>113.47806869999999</v>
+      </c>
+      <c r="I7" t="s">
+        <v>9</v>
+      </c>
+      <c r="J7">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A8">
         <v>78.692618038000006</v>
       </c>
-      <c r="B7">
+      <c r="B8">
         <v>-148.43002346700001</v>
       </c>
-      <c r="C7">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A8">
+      <c r="C8">
+        <v>0</v>
+      </c>
+      <c r="D8">
+        <f>COS(DEGREES(ATAN2(A8,B8)))*(SQRT(A8^2+B8^2)+$J$1)</f>
+        <v>143.12305128089912</v>
+      </c>
+      <c r="E8">
+        <f>SIN(DEGREES(ATAN2(A8,B8)))*(SQRT(A8^2+B8^2)+$J$1)</f>
+        <v>136.82029159503244</v>
+      </c>
+      <c r="F8">
+        <v>143.12305129999999</v>
+      </c>
+      <c r="G8" t="s">
+        <v>9</v>
+      </c>
+      <c r="H8">
+        <v>136.82029159999999</v>
+      </c>
+      <c r="I8" t="s">
+        <v>9</v>
+      </c>
+      <c r="J8">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A9">
         <v>44.944760873</v>
       </c>
-      <c r="B8">
+      <c r="B9">
         <v>-161.87639874300001</v>
       </c>
-      <c r="C8">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A9">
+      <c r="C9">
+        <v>0</v>
+      </c>
+      <c r="D9">
+        <f>COS(DEGREES(ATAN2(A9,B9)))*(SQRT(A9^2+B9^2)+$J$1)</f>
+        <v>120.6655393624545</v>
+      </c>
+      <c r="E9">
+        <f>SIN(DEGREES(ATAN2(A9,B9)))*(SQRT(A9^2+B9^2)+$J$1)</f>
+        <v>156.98352655705636</v>
+      </c>
+      <c r="F9">
+        <v>120.6655394</v>
+      </c>
+      <c r="G9" t="s">
+        <v>9</v>
+      </c>
+      <c r="H9">
+        <v>156.9835266</v>
+      </c>
+      <c r="I9" t="s">
+        <v>9</v>
+      </c>
+      <c r="J9">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A10">
         <v>9.0953366419999995</v>
       </c>
-      <c r="B9">
+      <c r="B10">
         <v>-167.753613527</v>
       </c>
-      <c r="C9">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A10">
+      <c r="C10">
+        <v>0</v>
+      </c>
+      <c r="D10">
+        <f>COS(DEGREES(ATAN2(A10,B10)))*(SQRT(A10^2+B10^2)+$J$1)</f>
+        <v>95.404391522959543</v>
+      </c>
+      <c r="E10">
+        <f>SIN(DEGREES(ATAN2(A10,B10)))*(SQRT(A10^2+B10^2)+$J$1)</f>
+        <v>173.49928552628324</v>
+      </c>
+      <c r="F10">
+        <v>95.404391520000004</v>
+      </c>
+      <c r="G10" t="s">
+        <v>9</v>
+      </c>
+      <c r="H10">
+        <v>173.49928550000001</v>
+      </c>
+      <c r="I10" t="s">
+        <v>9</v>
+      </c>
+      <c r="J10">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A11">
         <v>-27.179375421</v>
       </c>
-      <c r="B10">
+      <c r="B11">
         <v>-165.78685578700001</v>
       </c>
-      <c r="C10">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A11">
+      <c r="C11">
+        <v>0</v>
+      </c>
+      <c r="D11">
+        <f>COS(DEGREES(ATAN2(A11,B11)))*(SQRT(A11^2+B11^2)+$J$1)</f>
+        <v>67.926544637589984</v>
+      </c>
+      <c r="E11">
+        <f>SIN(DEGREES(ATAN2(A11,B11)))*(SQRT(A11^2+B11^2)+$J$1)</f>
+        <v>185.98382868845187</v>
+      </c>
+      <c r="F11">
+        <v>67.926544640000003</v>
+      </c>
+      <c r="G11" t="s">
+        <v>9</v>
+      </c>
+      <c r="H11">
+        <v>185.9838287</v>
+      </c>
+      <c r="I11" t="s">
+        <v>9</v>
+      </c>
+      <c r="J11">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A12">
         <v>-62.183210097</v>
       </c>
-      <c r="B11">
+      <c r="B12">
         <v>-156.068088929</v>
       </c>
-      <c r="C11">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A12">
+      <c r="C12">
+        <v>0</v>
+      </c>
+      <c r="D12">
+        <f>COS(DEGREES(ATAN2(A12,B12)))*(SQRT(A12^2+B12^2)+$J$1)</f>
+        <v>38.870440177271291</v>
+      </c>
+      <c r="E12">
+        <f>SIN(DEGREES(ATAN2(A12,B12)))*(SQRT(A12^2+B12^2)+$J$1)</f>
+        <v>194.14708053516645</v>
+      </c>
+      <c r="F12">
+        <v>38.870440180000003</v>
+      </c>
+      <c r="G12" t="s">
+        <v>9</v>
+      </c>
+      <c r="H12">
+        <v>194.14708049999999</v>
+      </c>
+      <c r="I12" t="s">
+        <v>9</v>
+      </c>
+      <c r="J12">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A13">
         <v>-94.279426981</v>
       </c>
-      <c r="B12">
+      <c r="B13">
         <v>-139.05175169</v>
       </c>
-      <c r="C12">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A13">
+      <c r="C13">
+        <v>0</v>
+      </c>
+      <c r="D13">
+        <f>COS(DEGREES(ATAN2(A13,B13)))*(SQRT(A13^2+B13^2)+$J$1)</f>
+        <v>8.9111900465788292</v>
+      </c>
+      <c r="E13">
+        <f>SIN(DEGREES(ATAN2(A13,B13)))*(SQRT(A13^2+B13^2)+$J$1)</f>
+        <v>197.79936979642568</v>
+      </c>
+      <c r="F13">
+        <v>8.9111900469999998</v>
+      </c>
+      <c r="G13" t="s">
+        <v>9</v>
+      </c>
+      <c r="H13">
+        <v>197.79936979999999</v>
+      </c>
+      <c r="I13" t="s">
+        <v>9</v>
+      </c>
+      <c r="J13">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A14">
         <v>-121.96724264300001</v>
       </c>
-      <c r="B13">
+      <c r="B14">
         <v>-115.533509087</v>
       </c>
-      <c r="C13">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A14">
+      <c r="C14">
+        <v>0</v>
+      </c>
+      <c r="F14">
+        <v>8.9111900469999998</v>
+      </c>
+      <c r="G14" t="s">
+        <v>9</v>
+      </c>
+      <c r="H14">
+        <v>197.79936979999999</v>
+      </c>
+      <c r="I14" t="s">
+        <v>9</v>
+      </c>
+      <c r="J14">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A15">
         <v>-143.95200559599999</v>
       </c>
-      <c r="B14">
+      <c r="B15">
         <v>-86.613048006</v>
       </c>
-      <c r="C14">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A15">
+      <c r="C15">
+        <v>0</v>
+      </c>
+      <c r="F15">
+        <v>-8.9111900469999998</v>
+      </c>
+      <c r="G15" t="s">
+        <v>9</v>
+      </c>
+      <c r="H15">
+        <v>197.79936979999999</v>
+      </c>
+      <c r="I15" t="s">
+        <v>9</v>
+      </c>
+      <c r="J15">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A16">
         <v>-159.205732759</v>
       </c>
-      <c r="B15">
+      <c r="B16">
         <v>-53.642657063000001</v>
       </c>
-      <c r="C15">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A16">
-        <v>-167.01517680200001</v>
-      </c>
-      <c r="B16">
-        <v>-18.163995095000001</v>
-      </c>
       <c r="C16">
         <v>0</v>
       </c>
-    </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="F16">
+        <v>-38.870440180000003</v>
+      </c>
+      <c r="G16" t="s">
+        <v>9</v>
+      </c>
+      <c r="H16">
+        <v>194.14708049999999</v>
+      </c>
+      <c r="I16" t="s">
+        <v>9</v>
+      </c>
+      <c r="J16">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>-167.01517680200001</v>
       </c>
       <c r="B17">
+        <v>-18.163995095000001</v>
+      </c>
+      <c r="C17">
+        <v>0</v>
+      </c>
+      <c r="F17">
+        <v>-67.926544640000003</v>
+      </c>
+      <c r="G17" t="s">
+        <v>9</v>
+      </c>
+      <c r="H17">
+        <v>185.9838287</v>
+      </c>
+      <c r="I17" t="s">
+        <v>9</v>
+      </c>
+      <c r="J17">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A18">
+        <v>-167.01517680200001</v>
+      </c>
+      <c r="B18">
         <v>18.163995095000001</v>
       </c>
-      <c r="C17">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A18">
+      <c r="C18">
+        <v>0</v>
+      </c>
+      <c r="F18">
+        <v>-95.404391520000004</v>
+      </c>
+      <c r="G18" t="s">
+        <v>9</v>
+      </c>
+      <c r="H18">
+        <v>173.49928550000001</v>
+      </c>
+      <c r="I18" t="s">
+        <v>9</v>
+      </c>
+      <c r="J18">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A19">
         <v>-159.205732759</v>
       </c>
-      <c r="B18">
+      <c r="B19">
         <v>53.642657063000001</v>
       </c>
-      <c r="C18">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A19">
+      <c r="C19">
+        <v>0</v>
+      </c>
+      <c r="F19">
+        <v>-120.6655394</v>
+      </c>
+      <c r="G19" t="s">
+        <v>9</v>
+      </c>
+      <c r="H19">
+        <v>156.9835266</v>
+      </c>
+      <c r="I19" t="s">
+        <v>9</v>
+      </c>
+      <c r="J19">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="20" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A20">
         <v>-143.95200559599999</v>
       </c>
-      <c r="B19">
+      <c r="B20">
         <v>86.613048006</v>
       </c>
-      <c r="C19">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A20">
+      <c r="C20">
+        <v>0</v>
+      </c>
+      <c r="F20">
+        <v>-143.12305129999999</v>
+      </c>
+      <c r="G20" t="s">
+        <v>9</v>
+      </c>
+      <c r="H20">
+        <v>136.82029159999999</v>
+      </c>
+      <c r="I20" t="s">
+        <v>9</v>
+      </c>
+      <c r="J20">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="21" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A21">
         <v>-121.96724264300001</v>
       </c>
-      <c r="B20">
+      <c r="B21">
         <v>115.533509087</v>
       </c>
-      <c r="C20">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A21">
+      <c r="C21">
+        <v>0</v>
+      </c>
+      <c r="F21">
+        <v>-162.25513219999999</v>
+      </c>
+      <c r="G21" t="s">
+        <v>9</v>
+      </c>
+      <c r="H21">
+        <v>113.47806869999999</v>
+      </c>
+      <c r="I21" t="s">
+        <v>9</v>
+      </c>
+      <c r="J21">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="22" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A22">
         <v>-94.279426981</v>
       </c>
-      <c r="B21">
+      <c r="B22">
         <v>139.05175169</v>
       </c>
-      <c r="C21">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A22">
+      <c r="C22">
+        <v>0</v>
+      </c>
+      <c r="D22">
+        <f>COS(DEGREES(ATAN2(A22,B22)))*(SQRT(A22^2+B22^2)+$J$1)</f>
+        <v>8.9111900465788292</v>
+      </c>
+      <c r="E22">
+        <f>SIN(DEGREES(ATAN2(A22,B22)))*(SQRT(A22^2+B22^2)+$J$1)</f>
+        <v>-197.79936979642568</v>
+      </c>
+      <c r="F22">
+        <v>-177.61725250000001</v>
+      </c>
+      <c r="G22" t="s">
+        <v>9</v>
+      </c>
+      <c r="H22">
+        <v>87.499209149999999</v>
+      </c>
+      <c r="I22" t="s">
+        <v>9</v>
+      </c>
+      <c r="J22">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="23" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A23">
         <v>-62.183210097</v>
       </c>
-      <c r="B22">
+      <c r="B23">
         <v>156.068088929</v>
       </c>
-      <c r="C22">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A23">
+      <c r="C23">
+        <v>0</v>
+      </c>
+      <c r="D23">
+        <f>COS(DEGREES(ATAN2(A23,B23)))*(SQRT(A23^2+B23^2)+$J$1)</f>
+        <v>38.870440177271291</v>
+      </c>
+      <c r="E23">
+        <f>SIN(DEGREES(ATAN2(A23,B23)))*(SQRT(A23^2+B23^2)+$J$1)</f>
+        <v>-194.14708053516645</v>
+      </c>
+      <c r="F23">
+        <v>-188.85247699999999</v>
+      </c>
+      <c r="G23" t="s">
+        <v>9</v>
+      </c>
+      <c r="H23">
+        <v>59.487325679999998</v>
+      </c>
+      <c r="I23" t="s">
+        <v>9</v>
+      </c>
+      <c r="J23">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="24" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A24">
         <v>-27.179375421</v>
       </c>
-      <c r="B23">
+      <c r="B24">
         <v>165.78685578700001</v>
       </c>
-      <c r="C23">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A24">
+      <c r="C24">
+        <v>0</v>
+      </c>
+      <c r="D24">
+        <f>COS(DEGREES(ATAN2(A24,B24)))*(SQRT(A24^2+B24^2)+$J$1)</f>
+        <v>67.926544637589984</v>
+      </c>
+      <c r="E24">
+        <f>SIN(DEGREES(ATAN2(A24,B24)))*(SQRT(A24^2+B24^2)+$J$1)</f>
+        <v>-185.98382868845187</v>
+      </c>
+      <c r="F24">
+        <v>-195.69975790000001</v>
+      </c>
+      <c r="G24" t="s">
+        <v>9</v>
+      </c>
+      <c r="H24">
+        <v>30.093267919999999</v>
+      </c>
+      <c r="I24" t="s">
+        <v>9</v>
+      </c>
+      <c r="J24">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="25" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A25">
         <v>9.0953366419999995</v>
       </c>
-      <c r="B24">
+      <c r="B25">
         <v>167.753613527</v>
       </c>
-      <c r="C24">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A25">
+      <c r="C25">
+        <v>0</v>
+      </c>
+      <c r="D25">
+        <f>COS(DEGREES(ATAN2(A25,B25)))*(SQRT(A25^2+B25^2)+$J$1)</f>
+        <v>95.404391522959543</v>
+      </c>
+      <c r="E25">
+        <f>SIN(DEGREES(ATAN2(A25,B25)))*(SQRT(A25^2+B25^2)+$J$1)</f>
+        <v>-173.49928552628324</v>
+      </c>
+      <c r="F25">
+        <v>-198</v>
+      </c>
+      <c r="G25" t="s">
+        <v>9</v>
+      </c>
+      <c r="H25">
+        <v>0</v>
+      </c>
+      <c r="I25" t="s">
+        <v>9</v>
+      </c>
+      <c r="J25">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="26" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A26">
         <v>44.944760873</v>
       </c>
-      <c r="B25">
+      <c r="B26">
         <v>161.87639874300001</v>
       </c>
-      <c r="C25">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A26">
+      <c r="C26">
+        <v>0</v>
+      </c>
+      <c r="D26">
+        <f>COS(DEGREES(ATAN2(A26,B26)))*(SQRT(A26^2+B26^2)+$J$1)</f>
+        <v>120.6655393624545</v>
+      </c>
+      <c r="E26">
+        <f>SIN(DEGREES(ATAN2(A26,B26)))*(SQRT(A26^2+B26^2)+$J$1)</f>
+        <v>-156.98352655705636</v>
+      </c>
+      <c r="F26">
+        <v>-198</v>
+      </c>
+      <c r="G26" t="s">
+        <v>9</v>
+      </c>
+      <c r="H26">
+        <v>0</v>
+      </c>
+      <c r="I26" t="s">
+        <v>9</v>
+      </c>
+      <c r="J26">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="27" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A27">
         <v>78.692618038000006</v>
       </c>
-      <c r="B26">
+      <c r="B27">
         <v>148.43002346700001</v>
       </c>
-      <c r="C26">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A27">
+      <c r="C27">
+        <v>0</v>
+      </c>
+      <c r="D27">
+        <f>COS(DEGREES(ATAN2(A27,B27)))*(SQRT(A27^2+B27^2)+$J$1)</f>
+        <v>143.12305128089912</v>
+      </c>
+      <c r="E27">
+        <f>SIN(DEGREES(ATAN2(A27,B27)))*(SQRT(A27^2+B27^2)+$J$1)</f>
+        <v>-136.82029159503244</v>
+      </c>
+      <c r="F27">
+        <v>-195.69975790000001</v>
+      </c>
+      <c r="G27" t="s">
+        <v>9</v>
+      </c>
+      <c r="H27">
+        <v>-30.093267919999999</v>
+      </c>
+      <c r="I27" t="s">
+        <v>9</v>
+      </c>
+      <c r="J27">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="28" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A28">
         <v>108.760895843</v>
       </c>
-      <c r="B27">
+      <c r="B28">
         <v>128.043225261</v>
       </c>
-      <c r="C27">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A28">
+      <c r="C28">
+        <v>0</v>
+      </c>
+      <c r="D28">
+        <f>COS(DEGREES(ATAN2(A28,B28)))*(SQRT(A28^2+B28^2)+$J$1)</f>
+        <v>162.25513217730688</v>
+      </c>
+      <c r="E28">
+        <f>SIN(DEGREES(ATAN2(A28,B28)))*(SQRT(A28^2+B28^2)+$J$1)</f>
+        <v>-113.47806872652541</v>
+      </c>
+      <c r="F28">
+        <v>-188.85247699999999</v>
+      </c>
+      <c r="G28" t="s">
+        <v>9</v>
+      </c>
+      <c r="H28">
+        <v>-59.487325679999998</v>
+      </c>
+      <c r="I28" t="s">
+        <v>9</v>
+      </c>
+      <c r="J28">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="29" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A29">
         <v>133.743635039</v>
       </c>
-      <c r="B28">
+      <c r="B29">
         <v>101.669268153</v>
       </c>
-      <c r="C28">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A29">
+      <c r="C29">
+        <v>0</v>
+      </c>
+      <c r="D29">
+        <f>COS(DEGREES(ATAN2(A29,B29)))*(SQRT(A29^2+B29^2)+$J$1)</f>
+        <v>177.61725253691722</v>
+      </c>
+      <c r="E29">
+        <f>SIN(DEGREES(ATAN2(A29,B29)))*(SQRT(A29^2+B29^2)+$J$1)</f>
+        <v>-87.499209147778302</v>
+      </c>
+      <c r="F29">
+        <v>-177.61725250000001</v>
+      </c>
+      <c r="G29" t="s">
+        <v>9</v>
+      </c>
+      <c r="H29">
+        <v>-87.499209149999999</v>
+      </c>
+      <c r="I29" t="s">
+        <v>9</v>
+      </c>
+      <c r="J29">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="30" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A30">
         <v>152.472670505</v>
       </c>
-      <c r="B29">
+      <c r="B30">
         <v>70.541369062000001</v>
       </c>
-      <c r="C29">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A30">
+      <c r="C30">
+        <v>0</v>
+      </c>
+      <c r="D30">
+        <f>COS(DEGREES(ATAN2(A30,B30)))*(SQRT(A30^2+B30^2)+$J$1)</f>
+        <v>188.85247703960047</v>
+      </c>
+      <c r="E30">
+        <f>SIN(DEGREES(ATAN2(A30,B30)))*(SQRT(A30^2+B30^2)+$J$1)</f>
+        <v>-59.487325676036477</v>
+      </c>
+      <c r="F30">
+        <v>-162.25513219999999</v>
+      </c>
+      <c r="G30" t="s">
+        <v>9</v>
+      </c>
+      <c r="H30">
+        <v>-113.47806869999999</v>
+      </c>
+      <c r="I30" t="s">
+        <v>9</v>
+      </c>
+      <c r="J30">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="31" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A31">
         <v>164.072253359</v>
       </c>
-      <c r="B30">
+      <c r="B31">
         <v>36.115033955000001</v>
       </c>
-      <c r="C30">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A31">
-        <v>168</v>
-      </c>
-      <c r="B31">
-        <v>0</v>
-      </c>
       <c r="C31">
         <v>0</v>
       </c>
-    </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D31">
+        <f>COS(DEGREES(ATAN2(A31,B31)))*(SQRT(A31^2+B31^2)+$J$1)</f>
+        <v>195.6997578580409</v>
+      </c>
+      <c r="E31">
+        <f>SIN(DEGREES(ATAN2(A31,B31)))*(SQRT(A31^2+B31^2)+$J$1)</f>
+        <v>-30.093267920778441</v>
+      </c>
+      <c r="F31">
+        <v>-143.12305129999999</v>
+      </c>
+      <c r="G31" t="s">
+        <v>9</v>
+      </c>
+      <c r="H31">
+        <v>-136.82029159999999</v>
+      </c>
+      <c r="I31" t="s">
+        <v>9</v>
+      </c>
+      <c r="J31">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="32" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A32">
         <v>168</v>
       </c>
@@ -12314,7 +13664,354 @@
         <v>0</v>
       </c>
       <c r="C32">
+        <v>0</v>
+      </c>
+      <c r="D32">
+        <f>COS(DEGREES(ATAN2(A32,B32)))*(SQRT(A32^2+B32^2)+$J$1)</f>
+        <v>198</v>
+      </c>
+      <c r="E32">
+        <f>SIN(DEGREES(ATAN2(A32,B32)))*(SQRT(A32^2+B32^2)+$J$1)</f>
+        <v>0</v>
+      </c>
+      <c r="F32">
+        <v>-120.6655394</v>
+      </c>
+      <c r="G32" t="s">
+        <v>9</v>
+      </c>
+      <c r="H32">
+        <v>-156.9835266</v>
+      </c>
+      <c r="I32" t="s">
+        <v>9</v>
+      </c>
+      <c r="J32">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="33" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A33">
+        <v>168</v>
+      </c>
+      <c r="B33">
+        <v>0</v>
+      </c>
+      <c r="C33">
         <v>130</v>
+      </c>
+      <c r="D33">
+        <f>COS(DEGREES(ATAN2(A33,B33)))*(SQRT(A33^2+B33^2)+$J$1)</f>
+        <v>198</v>
+      </c>
+      <c r="E33">
+        <f>SIN(DEGREES(ATAN2(A33,B33)))*(SQRT(A33^2+B33^2)+$J$1)</f>
+        <v>0</v>
+      </c>
+      <c r="F33">
+        <v>-95.404391520000004</v>
+      </c>
+      <c r="G33" t="s">
+        <v>9</v>
+      </c>
+      <c r="H33">
+        <v>-173.49928550000001</v>
+      </c>
+      <c r="I33" t="s">
+        <v>9</v>
+      </c>
+      <c r="J33">
+        <f t="shared" si="0"/>
+        <v>130</v>
+      </c>
+    </row>
+    <row r="34" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="F34">
+        <v>-67.926544640000003</v>
+      </c>
+      <c r="G34" t="s">
+        <v>9</v>
+      </c>
+      <c r="H34">
+        <v>-185.9838287</v>
+      </c>
+      <c r="I34" t="s">
+        <v>9</v>
+      </c>
+      <c r="J34">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="35" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="F35">
+        <v>-38.870440180000003</v>
+      </c>
+      <c r="G35" t="s">
+        <v>9</v>
+      </c>
+      <c r="H35">
+        <v>-194.14708049999999</v>
+      </c>
+      <c r="I35" t="s">
+        <v>9</v>
+      </c>
+      <c r="J35">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="36" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="F36">
+        <v>-8.9111900469999998</v>
+      </c>
+      <c r="G36" t="s">
+        <v>9</v>
+      </c>
+      <c r="H36">
+        <v>-197.79936979999999</v>
+      </c>
+      <c r="I36" t="s">
+        <v>9</v>
+      </c>
+      <c r="J36">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="37" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="F37">
+        <v>-8.9111900469999998</v>
+      </c>
+      <c r="G37" t="s">
+        <v>9</v>
+      </c>
+      <c r="H37">
+        <v>-197.79936979999999</v>
+      </c>
+      <c r="I37" t="s">
+        <v>9</v>
+      </c>
+      <c r="J37">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="38" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="F38">
+        <v>8.9111900469999998</v>
+      </c>
+      <c r="G38" t="s">
+        <v>9</v>
+      </c>
+      <c r="H38">
+        <v>-197.79936979999999</v>
+      </c>
+      <c r="I38" t="s">
+        <v>9</v>
+      </c>
+      <c r="J38">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="39" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="F39">
+        <v>38.870440180000003</v>
+      </c>
+      <c r="G39" t="s">
+        <v>9</v>
+      </c>
+      <c r="H39">
+        <v>-194.14708049999999</v>
+      </c>
+      <c r="I39" t="s">
+        <v>9</v>
+      </c>
+      <c r="J39">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="40" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="F40">
+        <v>67.926544640000003</v>
+      </c>
+      <c r="G40" t="s">
+        <v>9</v>
+      </c>
+      <c r="H40">
+        <v>-185.9838287</v>
+      </c>
+      <c r="I40" t="s">
+        <v>9</v>
+      </c>
+      <c r="J40">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="41" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="F41">
+        <v>95.404391520000004</v>
+      </c>
+      <c r="G41" t="s">
+        <v>9</v>
+      </c>
+      <c r="H41">
+        <v>-173.49928550000001</v>
+      </c>
+      <c r="I41" t="s">
+        <v>9</v>
+      </c>
+      <c r="J41">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="42" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="F42">
+        <v>120.6655394</v>
+      </c>
+      <c r="G42" t="s">
+        <v>9</v>
+      </c>
+      <c r="H42">
+        <v>-156.9835266</v>
+      </c>
+      <c r="I42" t="s">
+        <v>9</v>
+      </c>
+      <c r="J42">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="43" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="F43">
+        <v>143.12305129999999</v>
+      </c>
+      <c r="G43" t="s">
+        <v>9</v>
+      </c>
+      <c r="H43">
+        <v>-136.82029159999999</v>
+      </c>
+      <c r="I43" t="s">
+        <v>9</v>
+      </c>
+      <c r="J43">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="44" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="F44">
+        <v>162.25513219999999</v>
+      </c>
+      <c r="G44" t="s">
+        <v>9</v>
+      </c>
+      <c r="H44">
+        <v>-113.47806869999999</v>
+      </c>
+      <c r="I44" t="s">
+        <v>9</v>
+      </c>
+      <c r="J44">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="45" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="F45">
+        <v>177.61725250000001</v>
+      </c>
+      <c r="G45" t="s">
+        <v>9</v>
+      </c>
+      <c r="H45">
+        <v>-87.499209149999999</v>
+      </c>
+      <c r="I45" t="s">
+        <v>9</v>
+      </c>
+      <c r="J45">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="46" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="F46">
+        <v>188.85247699999999</v>
+      </c>
+      <c r="G46" t="s">
+        <v>9</v>
+      </c>
+      <c r="H46">
+        <v>-59.487325679999998</v>
+      </c>
+      <c r="I46" t="s">
+        <v>9</v>
+      </c>
+      <c r="J46">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="47" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="F47">
+        <v>195.69975790000001</v>
+      </c>
+      <c r="G47" t="s">
+        <v>9</v>
+      </c>
+      <c r="H47">
+        <v>-30.093267919999999</v>
+      </c>
+      <c r="I47" t="s">
+        <v>9</v>
+      </c>
+      <c r="J47">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="48" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="F48">
+        <v>198</v>
+      </c>
+      <c r="G48" t="s">
+        <v>9</v>
+      </c>
+      <c r="H48">
+        <v>0</v>
+      </c>
+      <c r="I48" t="s">
+        <v>9</v>
+      </c>
+      <c r="J48">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="49" spans="6:10" x14ac:dyDescent="0.25">
+      <c r="F49">
+        <v>198</v>
+      </c>
+      <c r="G49" t="s">
+        <v>9</v>
+      </c>
+      <c r="H49">
+        <v>0</v>
+      </c>
+      <c r="I49" t="s">
+        <v>9</v>
+      </c>
+      <c r="J49">
+        <f t="shared" si="0"/>
+        <v>0</v>
       </c>
     </row>
   </sheetData>
@@ -12869,26 +14566,44 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ADFEAEE7-D398-4588-A5CE-E2B51CDA9D3F}">
-  <dimension ref="A1:C44"/>
+  <dimension ref="A1:I45"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C6" sqref="C6"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A1">
-        <v>295</v>
-      </c>
-      <c r="B1">
-        <v>0</v>
-      </c>
-      <c r="C1">
-        <v>120</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" t="s">
+        <v>7</v>
+      </c>
+      <c r="H1">
+        <v>30</v>
+      </c>
+      <c r="I1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>295</v>
       </c>
@@ -12896,219 +14611,583 @@
         <v>0</v>
       </c>
       <c r="C2">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+        <v>120</v>
+      </c>
+      <c r="D2">
+        <f>COS(DEGREES(ATAN2(A2,B2)))*(SQRT(A2^2+B2^2)-$H$1)</f>
+        <v>265</v>
+      </c>
+      <c r="E2">
+        <f>SIN(DEGREES(ATAN2(A2,B2)))*(SQRT(A2^2+B2^2)-$H$1)</f>
+        <v>0</v>
+      </c>
+      <c r="F2">
+        <f>C2</f>
+        <v>120</v>
+      </c>
+      <c r="G2">
+        <v>265</v>
+      </c>
+      <c r="H2">
+        <v>0</v>
+      </c>
+      <c r="I2">
+        <f>C2</f>
+        <v>120</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3">
+        <v>295</v>
+      </c>
+      <c r="B3">
+        <v>0</v>
+      </c>
+      <c r="C3">
+        <v>0</v>
+      </c>
+      <c r="D3">
+        <f t="shared" ref="D3:D45" si="0">COS(DEGREES(ATAN2(A3,B3)))*(SQRT(A3^2+B3^2)-$H$1)</f>
+        <v>265</v>
+      </c>
+      <c r="E3">
+        <f t="shared" ref="E3:E45" si="1">SIN(DEGREES(ATAN2(A3,B3)))*(SQRT(A3^2+B3^2)-$H$1)</f>
+        <v>0</v>
+      </c>
+      <c r="G3">
+        <v>265</v>
+      </c>
+      <c r="H3">
+        <v>0</v>
+      </c>
+      <c r="I3">
+        <f t="shared" ref="I3:I45" si="2">C3</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A4">
         <v>291.17982747799999</v>
       </c>
-      <c r="B3">
+      <c r="B4">
         <v>47.321327853</v>
       </c>
-      <c r="C3">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A4">
+      <c r="C4">
+        <v>0</v>
+      </c>
+      <c r="D4">
+        <f t="shared" si="0"/>
+        <v>-260.02840455548545</v>
+      </c>
+      <c r="E4">
+        <f t="shared" si="1"/>
+        <v>51.090398552262521</v>
+      </c>
+      <c r="G4">
+        <v>260.02840455548545</v>
+      </c>
+      <c r="H4">
+        <v>51.090398552262521</v>
+      </c>
+      <c r="I4">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A5">
         <v>279.818250374</v>
       </c>
-      <c r="B4">
+      <c r="B5">
         <v>93.417058170999994</v>
       </c>
-      <c r="C4">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A5">
+      <c r="C5">
+        <v>0</v>
+      </c>
+      <c r="D5">
+        <f t="shared" si="0"/>
+        <v>245.30015981147619</v>
+      </c>
+      <c r="E5">
+        <f t="shared" si="1"/>
+        <v>-100.26381000234454</v>
+      </c>
+      <c r="G5">
+        <v>245.30015981147619</v>
+      </c>
+      <c r="H5">
+        <v>100.26381000234454</v>
+      </c>
+      <c r="I5">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A6">
         <v>261.209527568</v>
       </c>
-      <c r="B5">
+      <c r="B6">
         <v>137.09333575299999</v>
       </c>
-      <c r="C5">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A6">
+      <c r="C6">
+        <v>0</v>
+      </c>
+      <c r="D6">
+        <f t="shared" si="0"/>
+        <v>-221.36789125110025</v>
+      </c>
+      <c r="E6">
+        <f t="shared" si="1"/>
+        <v>145.67517538415743</v>
+      </c>
+      <c r="G6">
+        <v>221.36789125110025</v>
+      </c>
+      <c r="H6">
+        <v>145.67517538415743</v>
+      </c>
+      <c r="I6">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A7">
         <v>235.83561520399999</v>
       </c>
-      <c r="B6">
+      <c r="B7">
         <v>177.21896795000001</v>
       </c>
-      <c r="C6">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A7">
+      <c r="C7">
+        <v>0</v>
+      </c>
+      <c r="D7">
+        <f t="shared" si="0"/>
+        <v>189.12957287379737</v>
+      </c>
+      <c r="E7">
+        <f t="shared" si="1"/>
+        <v>-185.6205933200736</v>
+      </c>
+      <c r="G7">
+        <v>221.36789125110025</v>
+      </c>
+      <c r="H7">
+        <v>145.67517538415743</v>
+      </c>
+      <c r="I7">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A8">
         <v>204.35368428500001</v>
       </c>
-      <c r="B7">
+      <c r="B8">
         <v>212.75472196600001</v>
       </c>
-      <c r="C7">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A8">
+      <c r="C8">
+        <v>0</v>
+      </c>
+      <c r="D8">
+        <f t="shared" si="0"/>
+        <v>-149.79483395270174</v>
+      </c>
+      <c r="E8">
+        <f t="shared" si="1"/>
+        <v>218.60125278872061</v>
+      </c>
+      <c r="G8">
+        <v>189.12957287379737</v>
+      </c>
+      <c r="H8">
+        <v>185.6205933200736</v>
+      </c>
+      <c r="I8">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A9">
         <v>167.579100286</v>
       </c>
-      <c r="B8">
+      <c r="B9">
         <v>242.78024043900001</v>
       </c>
-      <c r="C8">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A9">
+      <c r="C9">
+        <v>0</v>
+      </c>
+      <c r="D9">
+        <f t="shared" si="0"/>
+        <v>104.83957190478087</v>
+      </c>
+      <c r="E9">
+        <f t="shared" si="1"/>
+        <v>-243.3796708089591</v>
+      </c>
+      <c r="G9">
+        <v>149.79483395270174</v>
+      </c>
+      <c r="H9">
+        <v>218.60125278872061</v>
+      </c>
+      <c r="I9">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A10">
         <v>126.464305614</v>
       </c>
-      <c r="B9">
+      <c r="B10">
         <v>266.51787820999999</v>
       </c>
-      <c r="C9">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A10">
+      <c r="C10">
+        <v>0</v>
+      </c>
+      <c r="D10">
+        <f t="shared" si="0"/>
+        <v>-55.95057447043088</v>
+      </c>
+      <c r="E10">
+        <f t="shared" si="1"/>
+        <v>259.02612458287138</v>
+      </c>
+      <c r="G10">
+        <v>104.83957190478087</v>
+      </c>
+      <c r="H10">
+        <v>243.3796708089591</v>
+      </c>
+      <c r="I10">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A11">
         <v>82.074151854999997</v>
       </c>
-      <c r="B10">
+      <c r="B11">
         <v>283.352842931</v>
       </c>
-      <c r="C10">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A11">
+      <c r="C11">
+        <v>0</v>
+      </c>
+      <c r="D11">
+        <f t="shared" si="0"/>
+        <v>4.9622289754635514</v>
+      </c>
+      <c r="E11">
+        <f t="shared" si="1"/>
+        <v>-264.95353608399574</v>
+      </c>
+      <c r="G11">
+        <v>55.95057447043088</v>
+      </c>
+      <c r="H11">
+        <v>259.02612458287138</v>
+      </c>
+      <c r="I11">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A12">
         <v>35.558320674999997</v>
       </c>
-      <c r="B11">
+      <c r="B12">
         <v>292.84911785899999</v>
       </c>
-      <c r="C11">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A12">
+      <c r="C12">
+        <v>0</v>
+      </c>
+      <c r="D12">
+        <f t="shared" si="0"/>
+        <v>46.212306686624778</v>
+      </c>
+      <c r="E12">
+        <f t="shared" si="1"/>
+        <v>260.93950009670795</v>
+      </c>
+      <c r="G12">
+        <v>4.9622289754635514</v>
+      </c>
+      <c r="H12">
+        <v>264.95353608399574</v>
+      </c>
+      <c r="I12">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A13">
         <v>-11.878452332</v>
       </c>
-      <c r="B12">
+      <c r="B13">
         <v>294.76075446099998</v>
       </c>
-      <c r="C12">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A13">
+      <c r="C13">
+        <v>0</v>
+      </c>
+      <c r="D13">
+        <f t="shared" si="0"/>
+        <v>-95.652888469194707</v>
+      </c>
+      <c r="E13">
+        <f t="shared" si="1"/>
+        <v>-247.13462915524158</v>
+      </c>
+      <c r="G13">
+        <v>-4.9622289754635514</v>
+      </c>
+      <c r="H13">
+        <v>264.95353608399574</v>
+      </c>
+      <c r="I13">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A14">
         <v>-59.007579663999998</v>
       </c>
-      <c r="B13">
+      <c r="B14">
         <v>289.038242352</v>
       </c>
-      <c r="C13">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A14">
+      <c r="C14">
+        <v>0</v>
+      </c>
+      <c r="D14">
+        <f t="shared" si="0"/>
+        <v>141.50443273194517</v>
+      </c>
+      <c r="E14">
+        <f t="shared" si="1"/>
+        <v>224.0569024086827</v>
+      </c>
+      <c r="G14">
+        <v>-55.95057447043088</v>
+      </c>
+      <c r="H14">
+        <v>259.02612458287138</v>
+      </c>
+      <c r="I14">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A15">
         <v>-104.60844167800001</v>
       </c>
-      <c r="B14">
+      <c r="B15">
         <v>275.82979159199999</v>
       </c>
-      <c r="C14">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A15">
+      <c r="C15">
+        <v>0</v>
+      </c>
+      <c r="D15">
+        <f t="shared" si="0"/>
+        <v>-182.04652196218319</v>
+      </c>
+      <c r="E15">
+        <f t="shared" si="1"/>
+        <v>-192.5722301928798</v>
+      </c>
+      <c r="G15">
+        <v>-104.83957190478087</v>
+      </c>
+      <c r="H15">
+        <v>243.3796708089591</v>
+      </c>
+      <c r="I15">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A16">
         <v>-147.5</v>
       </c>
-      <c r="B15">
+      <c r="B16">
         <v>255.477494116</v>
       </c>
-      <c r="C15">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A16">
+      <c r="C16">
+        <v>0</v>
+      </c>
+      <c r="D16">
+        <f t="shared" si="0"/>
+        <v>215.75795718313236</v>
+      </c>
+      <c r="E16">
+        <f t="shared" si="1"/>
+        <v>153.8619638246364</v>
+      </c>
+      <c r="G16">
+        <v>-149.79483395270174</v>
+      </c>
+      <c r="H16">
+        <v>218.60125278872061</v>
+      </c>
+      <c r="I16">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A17">
         <v>-186.57138580099999</v>
       </c>
-      <c r="B16">
+      <c r="B17">
         <v>228.50846373900001</v>
       </c>
-      <c r="C16">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A17">
+      <c r="C17">
+        <v>0</v>
+      </c>
+      <c r="D17">
+        <f t="shared" si="0"/>
+        <v>-241.37383558273379</v>
+      </c>
+      <c r="E17">
+        <f t="shared" si="1"/>
+        <v>-109.37856963837289</v>
+      </c>
+      <c r="G17">
+        <v>-189.12957287379737</v>
+      </c>
+      <c r="H17">
+        <v>185.6205933200736</v>
+      </c>
+      <c r="I17">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A18">
         <v>-220.81067071000001</v>
       </c>
-      <c r="B17">
+      <c r="B18">
         <v>195.62118418099999</v>
       </c>
-      <c r="C17">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A18">
+      <c r="C18">
+        <v>0</v>
+      </c>
+      <c r="D18">
+        <f t="shared" si="0"/>
+        <v>257.9330116449421</v>
+      </c>
+      <c r="E18">
+        <f t="shared" si="1"/>
+        <v>60.791130138940765</v>
+      </c>
+      <c r="G18">
+        <v>-189.12957287379737</v>
+      </c>
+      <c r="H18">
+        <v>185.6205933200736</v>
+      </c>
+      <c r="I18">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A19">
         <v>-249.33107523499999</v>
       </c>
-      <c r="B18">
+      <c r="B19">
         <v>157.66741870800001</v>
       </c>
-      <c r="C18">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A19">
+      <c r="C19">
+        <v>0</v>
+      </c>
+      <c r="D19">
+        <f t="shared" si="0"/>
+        <v>-264.81416063266533</v>
+      </c>
+      <c r="E19">
+        <f t="shared" si="1"/>
+        <v>-9.922717788671509</v>
+      </c>
+      <c r="G19">
+        <v>-221.36789125110025</v>
+      </c>
+      <c r="H19">
+        <v>145.67517538415743</v>
+      </c>
+      <c r="I19">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A20">
         <v>-271.39393587900003</v>
       </c>
-      <c r="B19">
+      <c r="B20">
         <v>115.630149909</v>
       </c>
-      <c r="C19">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A20">
+      <c r="C20">
+        <v>0</v>
+      </c>
+      <c r="D20">
+        <f t="shared" si="0"/>
+        <v>261.75909169734325</v>
+      </c>
+      <c r="E20">
+        <f t="shared" si="1"/>
+        <v>-41.318009555971962</v>
+      </c>
+      <c r="G20">
+        <v>-245.30015981147619</v>
+      </c>
+      <c r="H20">
+        <v>100.26381000234454</v>
+      </c>
+      <c r="I20">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A21">
         <v>-286.427836141</v>
       </c>
-      <c r="B20">
+      <c r="B21">
         <v>70.598120965000007</v>
       </c>
-      <c r="C20">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A21">
-        <v>-294.04340589999998</v>
-      </c>
-      <c r="B21">
-        <v>23.737637770999999</v>
-      </c>
       <c r="C21">
         <v>0</v>
       </c>
-    </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D21">
+        <f t="shared" si="0"/>
+        <v>-248.88243553964202</v>
+      </c>
+      <c r="E21">
+        <f t="shared" si="1"/>
+        <v>91.008424225669714</v>
+      </c>
+      <c r="G21">
+        <v>-260.02840455548545</v>
+      </c>
+      <c r="H21">
+        <v>51.090398552262521</v>
+      </c>
+      <c r="I21">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="22" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A22">
         <v>-294.04340589999998</v>
       </c>
@@ -13116,21 +15195,57 @@
         <v>23.737637770999999</v>
       </c>
       <c r="C22">
-        <v>120</v>
-      </c>
-    </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
+        <v>0</v>
+      </c>
+      <c r="D22">
+        <f t="shared" si="0"/>
+        <v>226.66734329809088</v>
+      </c>
+      <c r="E22">
+        <f t="shared" si="1"/>
+        <v>-137.28406856726849</v>
+      </c>
+      <c r="G22">
+        <v>-265</v>
+      </c>
+      <c r="H22">
+        <v>0</v>
+      </c>
+      <c r="I22">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="23" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A23">
         <v>-294.04340589999998</v>
       </c>
       <c r="B23">
-        <v>-23.737637770999999</v>
+        <v>23.737637770999999</v>
       </c>
       <c r="C23">
         <v>120</v>
       </c>
-    </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D23">
+        <f t="shared" si="0"/>
+        <v>226.66734329809088</v>
+      </c>
+      <c r="E23">
+        <f t="shared" si="1"/>
+        <v>-137.28406856726849</v>
+      </c>
+      <c r="G23">
+        <v>-265</v>
+      </c>
+      <c r="H23">
+        <v>0</v>
+      </c>
+      <c r="I23">
+        <f t="shared" si="2"/>
+        <v>120</v>
+      </c>
+    </row>
+    <row r="24" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A24">
         <v>-294.04340589999998</v>
       </c>
@@ -13138,219 +15253,579 @@
         <v>-23.737637770999999</v>
       </c>
       <c r="C24">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
+        <v>120</v>
+      </c>
+      <c r="D24">
+        <f t="shared" si="0"/>
+        <v>226.66734329809088</v>
+      </c>
+      <c r="E24">
+        <f t="shared" si="1"/>
+        <v>137.28406856726849</v>
+      </c>
+      <c r="G24">
+        <v>-265</v>
+      </c>
+      <c r="H24">
+        <v>0</v>
+      </c>
+      <c r="I24">
+        <f t="shared" si="2"/>
+        <v>120</v>
+      </c>
+    </row>
+    <row r="25" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A25">
+        <v>-294.04340589999998</v>
+      </c>
+      <c r="B25">
+        <v>-23.737637770999999</v>
+      </c>
+      <c r="C25">
+        <v>0</v>
+      </c>
+      <c r="D25">
+        <f t="shared" si="0"/>
+        <v>226.66734329809088</v>
+      </c>
+      <c r="E25">
+        <f t="shared" si="1"/>
+        <v>137.28406856726849</v>
+      </c>
+      <c r="G25">
+        <v>-265</v>
+      </c>
+      <c r="H25">
+        <v>0</v>
+      </c>
+      <c r="I25">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="26" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A26">
         <v>-286.427836141</v>
       </c>
-      <c r="B25">
+      <c r="B26">
         <v>-70.598120965000007</v>
       </c>
-      <c r="C25">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A26">
+      <c r="C26">
+        <v>0</v>
+      </c>
+      <c r="D26">
+        <f t="shared" si="0"/>
+        <v>-248.88243553964202</v>
+      </c>
+      <c r="E26">
+        <f t="shared" si="1"/>
+        <v>-91.008424225669714</v>
+      </c>
+      <c r="G26">
+        <v>-260.02840455548545</v>
+      </c>
+      <c r="H26">
+        <v>-51.090398550000003</v>
+      </c>
+      <c r="I26">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="27" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A27">
         <v>-271.39393587900003</v>
       </c>
-      <c r="B26">
+      <c r="B27">
         <v>-115.630149909</v>
       </c>
-      <c r="C26">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A27">
+      <c r="C27">
+        <v>0</v>
+      </c>
+      <c r="D27">
+        <f t="shared" si="0"/>
+        <v>261.75909169734325</v>
+      </c>
+      <c r="E27">
+        <f t="shared" si="1"/>
+        <v>41.318009555971962</v>
+      </c>
+      <c r="G27">
+        <v>-245.30015981147619</v>
+      </c>
+      <c r="H27">
+        <v>-100.26381000000001</v>
+      </c>
+      <c r="I27">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="28" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A28">
         <v>-249.33107523499999</v>
       </c>
-      <c r="B27">
+      <c r="B28">
         <v>-157.66741870800001</v>
       </c>
-      <c r="C27">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A28">
+      <c r="C28">
+        <v>0</v>
+      </c>
+      <c r="D28">
+        <f t="shared" si="0"/>
+        <v>-264.81416063266533</v>
+      </c>
+      <c r="E28">
+        <f t="shared" si="1"/>
+        <v>9.922717788671509</v>
+      </c>
+      <c r="G28">
+        <v>-221.36789125110025</v>
+      </c>
+      <c r="H28">
+        <v>-145.6751754</v>
+      </c>
+      <c r="I28">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="29" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A29">
         <v>-220.81067071000001</v>
       </c>
-      <c r="B28">
+      <c r="B29">
         <v>-195.62118418099999</v>
       </c>
-      <c r="C28">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A29">
+      <c r="C29">
+        <v>0</v>
+      </c>
+      <c r="D29">
+        <f t="shared" si="0"/>
+        <v>257.9330116449421</v>
+      </c>
+      <c r="E29">
+        <f t="shared" si="1"/>
+        <v>-60.791130138940765</v>
+      </c>
+      <c r="G29">
+        <v>-221.36789125110025</v>
+      </c>
+      <c r="H29">
+        <v>-145.6751754</v>
+      </c>
+      <c r="I29">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="30" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A30">
         <v>-186.57138580099999</v>
       </c>
-      <c r="B29">
+      <c r="B30">
         <v>-228.50846373900001</v>
       </c>
-      <c r="C29">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A30">
+      <c r="C30">
+        <v>0</v>
+      </c>
+      <c r="D30">
+        <f t="shared" si="0"/>
+        <v>-241.37383558273379</v>
+      </c>
+      <c r="E30">
+        <f t="shared" si="1"/>
+        <v>109.37856963837289</v>
+      </c>
+      <c r="G30">
+        <v>-189.12957287379737</v>
+      </c>
+      <c r="H30">
+        <v>-185.6205933</v>
+      </c>
+      <c r="I30">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="31" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A31">
         <v>-147.5</v>
       </c>
-      <c r="B30">
+      <c r="B31">
         <v>-255.477494116</v>
       </c>
-      <c r="C30">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A31">
+      <c r="C31">
+        <v>0</v>
+      </c>
+      <c r="D31">
+        <f t="shared" si="0"/>
+        <v>215.75795718313236</v>
+      </c>
+      <c r="E31">
+        <f t="shared" si="1"/>
+        <v>-153.8619638246364</v>
+      </c>
+      <c r="G31">
+        <v>-149.79483395270174</v>
+      </c>
+      <c r="H31">
+        <v>-218.6012528</v>
+      </c>
+      <c r="I31">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="32" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A32">
         <v>-104.60844167800001</v>
       </c>
-      <c r="B31">
+      <c r="B32">
         <v>-275.82979159199999</v>
       </c>
-      <c r="C31">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A32">
+      <c r="C32">
+        <v>0</v>
+      </c>
+      <c r="D32">
+        <f t="shared" si="0"/>
+        <v>-182.04652196218319</v>
+      </c>
+      <c r="E32">
+        <f t="shared" si="1"/>
+        <v>192.5722301928798</v>
+      </c>
+      <c r="G32">
+        <v>-104.83957190478087</v>
+      </c>
+      <c r="H32">
+        <v>-243.37967080000001</v>
+      </c>
+      <c r="I32">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="33" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A33">
         <v>-59.007579663999998</v>
       </c>
-      <c r="B32">
+      <c r="B33">
         <v>-289.038242352</v>
       </c>
-      <c r="C32">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A33">
+      <c r="C33">
+        <v>0</v>
+      </c>
+      <c r="D33">
+        <f t="shared" si="0"/>
+        <v>141.50443273194517</v>
+      </c>
+      <c r="E33">
+        <f t="shared" si="1"/>
+        <v>-224.0569024086827</v>
+      </c>
+      <c r="G33">
+        <v>-55.95057447043088</v>
+      </c>
+      <c r="H33">
+        <v>-259.0261246</v>
+      </c>
+      <c r="I33">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="34" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A34">
         <v>-11.878452332</v>
       </c>
-      <c r="B33">
+      <c r="B34">
         <v>-294.76075446099998</v>
       </c>
-      <c r="C33">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A34">
+      <c r="C34">
+        <v>0</v>
+      </c>
+      <c r="D34">
+        <f t="shared" si="0"/>
+        <v>-95.652888469194707</v>
+      </c>
+      <c r="E34">
+        <f t="shared" si="1"/>
+        <v>247.13462915524158</v>
+      </c>
+      <c r="G34">
+        <v>-4.9622289754635514</v>
+      </c>
+      <c r="H34">
+        <v>-264.95353610000001</v>
+      </c>
+      <c r="I34">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="35" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A35">
         <v>35.558320674999997</v>
       </c>
-      <c r="B34">
+      <c r="B35">
         <v>-292.84911785899999</v>
       </c>
-      <c r="C34">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A35">
+      <c r="C35">
+        <v>0</v>
+      </c>
+      <c r="D35">
+        <f t="shared" si="0"/>
+        <v>46.212306686624778</v>
+      </c>
+      <c r="E35">
+        <f t="shared" si="1"/>
+        <v>-260.93950009670795</v>
+      </c>
+      <c r="G35">
+        <v>4.9622289750000004</v>
+      </c>
+      <c r="H35">
+        <v>-264.95353610000001</v>
+      </c>
+      <c r="I35">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="36" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A36">
         <v>82.074151854999997</v>
       </c>
-      <c r="B35">
+      <c r="B36">
         <v>-283.352842931</v>
       </c>
-      <c r="C35">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="36" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A36">
+      <c r="C36">
+        <v>0</v>
+      </c>
+      <c r="D36">
+        <f t="shared" si="0"/>
+        <v>4.9622289754635514</v>
+      </c>
+      <c r="E36">
+        <f t="shared" si="1"/>
+        <v>264.95353608399574</v>
+      </c>
+      <c r="G36">
+        <v>55.950574469999999</v>
+      </c>
+      <c r="H36">
+        <v>-259.0261246</v>
+      </c>
+      <c r="I36">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="37" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A37">
         <v>126.464305614</v>
       </c>
-      <c r="B36">
+      <c r="B37">
         <v>-266.51787820999999</v>
       </c>
-      <c r="C36">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="37" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A37">
+      <c r="C37">
+        <v>0</v>
+      </c>
+      <c r="D37">
+        <f t="shared" si="0"/>
+        <v>-55.95057447043088</v>
+      </c>
+      <c r="E37">
+        <f t="shared" si="1"/>
+        <v>-259.02612458287138</v>
+      </c>
+      <c r="G37">
+        <v>104.8395719</v>
+      </c>
+      <c r="H37">
+        <v>-243.37967080000001</v>
+      </c>
+      <c r="I37">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="38" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A38">
         <v>167.579100286</v>
       </c>
-      <c r="B37">
+      <c r="B38">
         <v>-242.78024043900001</v>
       </c>
-      <c r="C37">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="38" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A38">
+      <c r="C38">
+        <v>0</v>
+      </c>
+      <c r="D38">
+        <f t="shared" si="0"/>
+        <v>104.83957190478087</v>
+      </c>
+      <c r="E38">
+        <f t="shared" si="1"/>
+        <v>243.3796708089591</v>
+      </c>
+      <c r="G38">
+        <v>149.79483400000001</v>
+      </c>
+      <c r="H38">
+        <v>-218.6012528</v>
+      </c>
+      <c r="I38">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="39" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A39">
         <v>204.35368428500001</v>
       </c>
-      <c r="B38">
+      <c r="B39">
         <v>-212.75472196600001</v>
       </c>
-      <c r="C38">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="39" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A39">
+      <c r="C39">
+        <v>0</v>
+      </c>
+      <c r="D39">
+        <f t="shared" si="0"/>
+        <v>-149.79483395270174</v>
+      </c>
+      <c r="E39">
+        <f t="shared" si="1"/>
+        <v>-218.60125278872061</v>
+      </c>
+      <c r="G39">
+        <v>189.1295729</v>
+      </c>
+      <c r="H39">
+        <v>-185.6205933</v>
+      </c>
+      <c r="I39">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="40" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A40">
         <v>235.83561520399999</v>
       </c>
-      <c r="B39">
+      <c r="B40">
         <v>-177.21896795000001</v>
       </c>
-      <c r="C39">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="40" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A40">
+      <c r="C40">
+        <v>0</v>
+      </c>
+      <c r="D40">
+        <f t="shared" si="0"/>
+        <v>189.12957287379737</v>
+      </c>
+      <c r="E40">
+        <f t="shared" si="1"/>
+        <v>185.6205933200736</v>
+      </c>
+      <c r="G40">
+        <v>189.1295729</v>
+      </c>
+      <c r="H40">
+        <v>-185.6205933</v>
+      </c>
+      <c r="I40">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="41" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A41">
         <v>261.209527568</v>
       </c>
-      <c r="B40">
+      <c r="B41">
         <v>-137.09333575299999</v>
       </c>
-      <c r="C40">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="41" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A41">
+      <c r="C41">
+        <v>0</v>
+      </c>
+      <c r="D41">
+        <f t="shared" si="0"/>
+        <v>-221.36789125110025</v>
+      </c>
+      <c r="E41">
+        <f t="shared" si="1"/>
+        <v>-145.67517538415743</v>
+      </c>
+      <c r="G41">
+        <v>221.3678913</v>
+      </c>
+      <c r="H41">
+        <v>-145.6751754</v>
+      </c>
+      <c r="I41">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="42" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A42">
         <v>279.818250374</v>
       </c>
-      <c r="B41">
+      <c r="B42">
         <v>-93.417058170999994</v>
       </c>
-      <c r="C41">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="42" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A42">
+      <c r="C42">
+        <v>0</v>
+      </c>
+      <c r="D42">
+        <f t="shared" si="0"/>
+        <v>245.30015981147619</v>
+      </c>
+      <c r="E42">
+        <f t="shared" si="1"/>
+        <v>100.26381000234454</v>
+      </c>
+      <c r="G42">
+        <v>245.30015979999999</v>
+      </c>
+      <c r="H42">
+        <v>-100.26381000000001</v>
+      </c>
+      <c r="I42">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="43" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A43">
         <v>291.17982747799999</v>
       </c>
-      <c r="B42">
+      <c r="B43">
         <v>-47.321327853</v>
       </c>
-      <c r="C42">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="43" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A43">
-        <v>295</v>
-      </c>
-      <c r="B43">
-        <v>0</v>
-      </c>
       <c r="C43">
         <v>0</v>
       </c>
-    </row>
-    <row r="44" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D43">
+        <f t="shared" si="0"/>
+        <v>-260.02840455548545</v>
+      </c>
+      <c r="E43">
+        <f t="shared" si="1"/>
+        <v>-51.090398552262521</v>
+      </c>
+      <c r="G43">
+        <v>260.02840459999999</v>
+      </c>
+      <c r="H43">
+        <v>-51.090398550000003</v>
+      </c>
+      <c r="I43">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="44" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A44">
         <v>295</v>
       </c>
@@ -13358,6 +15833,53 @@
         <v>0</v>
       </c>
       <c r="C44">
+        <v>0</v>
+      </c>
+      <c r="D44">
+        <f t="shared" si="0"/>
+        <v>265</v>
+      </c>
+      <c r="E44">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="G44">
+        <v>265</v>
+      </c>
+      <c r="H44">
+        <v>0</v>
+      </c>
+      <c r="I44">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="45" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A45">
+        <v>295</v>
+      </c>
+      <c r="B45">
+        <v>0</v>
+      </c>
+      <c r="C45">
+        <v>120</v>
+      </c>
+      <c r="D45">
+        <f t="shared" si="0"/>
+        <v>265</v>
+      </c>
+      <c r="E45">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="G45">
+        <v>265</v>
+      </c>
+      <c r="H45">
+        <v>0</v>
+      </c>
+      <c r="I45">
+        <f t="shared" si="2"/>
         <v>120</v>
       </c>
     </row>

</xml_diff>